<commit_message>
updated batching of commands
</commit_message>
<xml_diff>
--- a/LINUX-ULTIMATE-GUIDE-SDAS/LINUX-COMMANDS.xlsx
+++ b/LINUX-ULTIMATE-GUIDE-SDAS/LINUX-COMMANDS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t xml:space="preserve">LINUX COMMAND</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t xml:space="preserve">ps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ls; who</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batching commands</t>
   </si>
 </sst>
 </file>
@@ -41,11 +53,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,6 +74,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,7 +129,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -131,17 +150,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="20.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -151,6 +170,36 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -160,6 +209,22 @@
     <row r="3" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -167,8 +232,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>